<commit_message>
Try to find why entropy is non-zero
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/debug_max_rew_mlp_5x200_small_batch_30k_epochs_eps_1e_12/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/debug_max_rew_mlp_5x200_small_batch_30k_epochs_eps_1e_12/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C373"/>
+  <dimension ref="A1:C376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5281,6 +5281,45 @@
         <v>15.52078786973544</v>
       </c>
     </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>[-6, 2, 0]</t>
+        </is>
+      </c>
+      <c r="C374" t="n">
+        <v>14.63151245515743</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>[-6, 2, 1]</t>
+        </is>
+      </c>
+      <c r="C375" t="n">
+        <v>14.74881737628981</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>[-7, 2, 1]</t>
+        </is>
+      </c>
+      <c r="C376" t="n">
+        <v>14.60931055454155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>